<commit_message>
Reprotect french and spanish databooks and some missed english sheets
</commit_message>
<xml_diff>
--- a/inputs/en/demo_demo_input.xlsx
+++ b/inputs/en/demo_demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1BF111-0A78-4CFF-BDCE-42A823482AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392020E7-7BB3-45E3-97CD-922E40E0F044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -5103,7 +5103,7 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -6528,7 +6528,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -6763,6 +6763,7 @@
       <c r="A19" s="36"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="FfHkqiZB4+MSNcSvC5AmHSBrL24DJqGBCUSbb1SXht/pvNfKrCwYwGQ0Nh0eFgbT4CtkrPtcdyerMXuqOASMgw==" saltValue="ujhgKiubLrCdAofmJLql6w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -8676,6 +8677,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="IEixURlTGTRJqZbHQmFhXvPIjUQmIm34YSzPBaRbABxdBmAg46d3JCYkT785QfIT3fChPybYBTXc2AW44XuyhA==" saltValue="fuFHWbJUOjdjm3xu1A1z1g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8688,7 +8690,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8880,6 +8882,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="HXM9d/yv0bR0otidlXI4b2tbsdUffgeJ2Wne/gEk97Pr2tTSdJnaP6hu45vmaWFjkHMXK2/VO+Xb1nLy35zSiA==" saltValue="tief35b+X1G5h293iqdAaA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -8893,8 +8896,8 @@
   </sheetPr>
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -10693,7 +10696,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Ap4P7JcBDpqTQtm6MYlYh14ybeQbemn6kklmftvLaZMGfb54sZfIKGNzDwetHNmHnka94h7SmhfC3Pd6f08CsA==" saltValue="aKkZemS/2Ya4OcDxk4iN8Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16742,6 +16745,42 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="tLFUmDyoH82P3agTzdNhIl/nrPXW114misPcwvY90QMxHUTQPj6nXWoXArIchS0+Y1PkNffvDNQ/0vLhBaHAnA==" saltValue="GmZrDncYr09T1PgEJ065qQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="45">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
     <mergeCell ref="B151:B153"/>
@@ -16751,42 +16790,6 @@
     <mergeCell ref="B134:B136"/>
     <mergeCell ref="B137:B139"/>
     <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -37130,6 +37133,7 @@
       <c r="K14" s="23"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="plogBhsuuJTsWPM2YhbeA1zjOmcXt4sZJzWkbAiBkI+j9As/GpEAx8GRXUW80IMb1WerNe/mHd+FIFLokb/7Jw==" saltValue="vtKvMzIczBBv/AXJ1k8ntg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="193" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>